<commit_message>
pregnancy tests data acquisitions
</commit_message>
<xml_diff>
--- a/metadata/STR-NHANES-2009-2010.xlsx
+++ b/metadata/STR-NHANES-2009-2010.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrique/git/nhanes-hadatac/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7981A9-685E-2846-8187-DC5D1A055A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B284698-2588-8147-B77F-0062F7E11893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="24280" windowHeight="16760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1120" yWindow="-19300" windowWidth="24280" windowHeight="16760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InfoSheet" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
   <si>
     <t xml:space="preserve">Property </t>
   </si>
@@ -169,6 +169,12 @@
   </si>
   <si>
     <t>nhanes-kb:DPL-TOSOH-G7-AUTOMATED-HPLC-ANALYZER</t>
+  </si>
+  <si>
+    <t>nhanes-kb:DPL-BECKMAN-COULTER-ICON-25-HCG-URINE-SERUM-TEST-KIT</t>
+  </si>
+  <si>
+    <t>NHANES-2009-2010-UCPREG_F</t>
   </si>
 </sst>
 </file>
@@ -243,7 +249,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -260,6 +266,7 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1542,17 +1549,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="29.6640625" style="5" customWidth="1"/>
     <col min="2" max="2" width="42.83203125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="55.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5" style="5" customWidth="1"/>
     <col min="5" max="5" width="22.83203125" style="5" customWidth="1"/>
     <col min="6" max="6" width="65.1640625" style="5" customWidth="1"/>
@@ -1705,6 +1712,24 @@
         <v>16</v>
       </c>
     </row>
+    <row r="9" spans="1:6" s="14" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" xr:uid="{4CBF1F59-E6CF-9C4E-ADAE-AD0B7423F61E}"/>
@@ -1714,6 +1739,7 @@
     <hyperlink ref="E7" r:id="rId5" xr:uid="{8FA29C4B-5D62-C241-B5A9-3548E5889E53}"/>
     <hyperlink ref="E2" r:id="rId6" xr:uid="{2764579B-87E0-6E49-8E4D-86FCABC15967}"/>
     <hyperlink ref="E8" r:id="rId7" xr:uid="{F94762BC-A13D-FF42-A2B5-42F93E20FADB}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{7A6F59F2-8521-B642-AFB2-1D8F3F36A9C9}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05278" bottom="1.05278" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait"/>

</xml_diff>